<commit_message>
Add several test cases,fix dates and borders
</commit_message>
<xml_diff>
--- a/Documents/QADocumentation.xlsx
+++ b/Documents/QADocumentation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kokster\Desktop\Maze-Game-main\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kokster\Maze-Game\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE623B9B-5903-4CD9-BFE7-BA1B612B35B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11070865-FC05-493C-9790-D439854D4A30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10416" xr2:uid="{DBAA5927-6D5D-4FAC-ABB9-E1D0AB0BFC4A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
   <si>
     <t>ID</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Test Menu</t>
   </si>
   <si>
-    <t>Ivaylo</t>
-  </si>
-  <si>
     <t>Manually</t>
   </si>
   <si>
@@ -96,12 +93,6 @@
     <t>Test Exit option</t>
   </si>
   <si>
-    <t>6.11.2021</t>
-  </si>
-  <si>
-    <t>05.11.2021</t>
-  </si>
-  <si>
     <t>Working without a problem</t>
   </si>
   <si>
@@ -115,6 +106,39 @@
   </si>
   <si>
     <t>Works well.</t>
+  </si>
+  <si>
+    <t>06.11.2021</t>
+  </si>
+  <si>
+    <t>Colours look perfect</t>
+  </si>
+  <si>
+    <t>Test winning message</t>
+  </si>
+  <si>
+    <t>08.11.2021</t>
+  </si>
+  <si>
+    <t>Message works perfect</t>
+  </si>
+  <si>
+    <t>Test maze end</t>
+  </si>
+  <si>
+    <t>07.11.2021</t>
+  </si>
+  <si>
+    <t>End works properly</t>
+  </si>
+  <si>
+    <t>Test walls stability</t>
+  </si>
+  <si>
+    <t>Everything passes</t>
+  </si>
+  <si>
+    <t>Ivaylo Markov</t>
   </si>
 </sst>
 </file>
@@ -145,7 +169,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -170,7 +194,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -182,6 +208,17 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -189,7 +226,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -204,37 +243,44 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,17 +595,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{008AC763-BDFA-48BE-AEE6-487A8BF938A1}">
-  <dimension ref="A2:H9"/>
+  <dimension ref="A2:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
@@ -596,182 +642,268 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
+      <c r="F5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="6" t="s">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
         <v>10</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="B12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
-        <v>2</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
-        <v>5</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
-        <v>3</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
-        <v>7</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="G12" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H9">
-    <sortCondition ref="E3:E9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A9">
+    <sortCondition ref="A3:A9"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add some style to the table
</commit_message>
<xml_diff>
--- a/Documents/QADocumentation.xlsx
+++ b/Documents/QADocumentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kokster\Maze-Game\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\Maze-Game\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6105D4A0-132B-44FC-ABEA-11D90265E191}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FC1708-8E84-469B-BA15-3EC4EDB31BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10416" xr2:uid="{DBAA5927-6D5D-4FAC-ABB9-E1D0AB0BFC4A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DBAA5927-6D5D-4FAC-ABB9-E1D0AB0BFC4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -190,35 +190,45 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="9"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -241,11 +251,109 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -256,15 +364,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -274,23 +373,295 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -301,6 +672,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E502F936-C1F3-449E-96AC-A5C29184F038}" name="Table1" displayName="Table1" ref="A2:H16" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+  <autoFilter ref="A2:H16" xr:uid="{E502F936-C1F3-449E-96AC-A5C29184F038}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{DF40DFB1-27D3-479E-B94D-F304A734867C}" name="ID" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{F9EA40B7-1723-47B1-B723-6E25B6C83C46}" name="Test Name" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{D9A5CFB6-11CE-40DD-9DC4-0B01D72A9F46}" name="Responsibility" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{A4D30B2C-242E-4FC9-862E-E3DC3E40B620}" name="Resources" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{1C02EAD6-4B4C-48D9-A059-B6620CE5242A}" name="Deadline" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{AC0A1A4F-1220-48F4-B424-4AA3FBED8C97}" name="Status" dataDxfId="3" dataCellStyle="Good"/>
+    <tableColumn id="7" xr3:uid="{104374D7-86C0-4F09-B5AD-024862C7FEBE}" name="Date completed" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{23E139FC-1E35-4E54-B2FF-E16D98201260}" name="Comments" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -603,51 +991,51 @@
   <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" customWidth="1"/>
-    <col min="8" max="8" width="29.33203125" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="53.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+    <row r="3" spans="1:8" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -662,18 +1050,18 @@
       <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="9" t="s">
         <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -688,18 +1076,18 @@
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -714,18 +1102,18 @@
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -740,18 +1128,18 @@
       <c r="E6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -766,44 +1154,44 @@
       <c r="E7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
+    <row r="8" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
         <v>6</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="6" t="s">
         <v>37</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="17" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -818,21 +1206,21 @@
       <c r="E9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
         <v>8</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="7" t="s">
         <v>40</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -844,18 +1232,18 @@
       <c r="E10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="12">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -870,21 +1258,21 @@
       <c r="E11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="12">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
         <v>10</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -893,24 +1281,24 @@
       <c r="D12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="12">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
         <v>11</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -919,24 +1307,24 @@
       <c r="D13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="12">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="14">
         <v>12</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -945,24 +1333,24 @@
       <c r="D14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="12">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
         <v>13</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -971,42 +1359,42 @@
       <c r="D15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="12">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="23">
         <v>14</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="28" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1014,8 +1402,11 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A9">
     <sortCondition ref="A3:A9"/>
   </sortState>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>